<commit_message>
Merchant Admin - Build combo and options functions for Product Management
</commit_message>
<xml_diff>
--- a/doc/SQL_design.xlsx
+++ b/doc/SQL_design.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Downloads\mySite_Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Downloads\mySite_Update\my-online-ordering\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="4980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="220">
   <si>
     <t>item_id</t>
   </si>
@@ -131,9 +131,6 @@
     <t>選項 ID</t>
   </si>
   <si>
-    <t>所屬商品</t>
-  </si>
-  <si>
     <t>選項名稱（如：加珍珠）</t>
   </si>
   <si>
@@ -143,12 +140,6 @@
     <t>加價金額</t>
   </si>
   <si>
-    <t>is_required</t>
-  </si>
-  <si>
-    <t>是否必選</t>
-  </si>
-  <si>
     <t>group_name</t>
   </si>
   <si>
@@ -518,37 +509,19 @@
     <t>套餐商品 ID</t>
   </si>
   <si>
-    <t>商品選項群組</t>
-  </si>
-  <si>
     <t>option_group_id</t>
   </si>
   <si>
     <t>選項群組 ID</t>
   </si>
   <si>
-    <t>is_template</t>
-  </si>
-  <si>
-    <t>是否為範本</t>
-  </si>
-  <si>
     <t>選項群組名（如：甜度、辣度）</t>
   </si>
   <si>
-    <t>template_name</t>
-  </si>
-  <si>
-    <t>範本名稱</t>
-  </si>
-  <si>
     <t>所屬選項群組 ID</t>
   </si>
   <si>
     <t>default_option_id</t>
-  </si>
-  <si>
-    <t>item_option_group</t>
   </si>
   <si>
     <t>item_option_default</t>
@@ -671,10 +644,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>是否多選</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>INT (CPK, FK)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -765,6 +734,46 @@
   </si>
   <si>
     <t>inventory</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>option_group</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>選項群組</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否多選 (單選為必選)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_universal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否通用</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>通用群組內部名稱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>universal_name</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>item_option_group</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品選項群組</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT (CPK FK)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -862,7 +871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -908,6 +917,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1191,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.2"/>
@@ -1239,46 +1251,46 @@
   <sheetData>
     <row r="1" spans="1:47" ht="56.55" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F1" s="11"/>
       <c r="G1" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="J1" s="11"/>
       <c r="K1" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="N1" s="11"/>
       <c r="O1" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="R1" s="11"/>
       <c r="S1" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="V1" s="11"/>
       <c r="W1" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:47" ht="40.200000000000003" thickBot="1">
@@ -1289,13 +1301,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>5</v>
@@ -1305,7 +1317,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>5</v>
@@ -1314,7 +1326,7 @@
         <v>3</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>5</v>
@@ -1323,19 +1335,19 @@
         <v>3</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="X2" s="4"/>
     </row>
@@ -1347,13 +1359,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>2</v>
@@ -1363,7 +1375,7 @@
         <v>14</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>26</v>
@@ -1372,19 +1384,19 @@
         <v>0</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>3</v>
@@ -1405,7 +1417,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -1427,43 +1439,43 @@
         <v>27</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="X4" s="4"/>
     </row>
     <row r="5" spans="1:47" ht="40.200000000000003" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
@@ -1485,43 +1497,43 @@
         <v>30</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="X5" s="4"/>
     </row>
     <row r="6" spans="1:47" ht="79.8" thickBot="1">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -1530,7 +1542,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="3" t="s">
@@ -1543,7 +1555,7 @@
         <v>32</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>22</v>
@@ -1552,22 +1564,22 @@
         <v>25</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:47" ht="27" thickBot="1">
@@ -1593,22 +1605,22 @@
       <c r="I7" s="1"/>
       <c r="J7" s="4"/>
       <c r="Q7" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="V7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:47" ht="79.8" thickBot="1">
@@ -1632,36 +1644,36 @@
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="11" t="s">
-        <v>174</v>
+        <v>210</v>
       </c>
       <c r="J8" s="11"/>
-      <c r="K8" s="11" t="s">
-        <v>164</v>
+      <c r="K8" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N8" s="11"/>
       <c r="O8" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="V8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="Y8" s="3"/>
       <c r="Z8" s="4"/>
@@ -1669,20 +1681,20 @@
     </row>
     <row r="9" spans="1:47" ht="79.8" thickBot="1">
       <c r="E9" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>5</v>
@@ -1691,65 +1703,65 @@
         <v>3</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="V9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:47" ht="93" thickBot="1">
       <c r="A10" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="7"/>
@@ -1757,13 +1769,13 @@
     </row>
     <row r="11" spans="1:47" ht="40.200000000000003" thickBot="1">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>19</v>
@@ -1776,13 +1788,13 @@
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>6</v>
@@ -1791,14 +1803,14 @@
         <v>7</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Q11" s="10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R11" s="11"/>
       <c r="S11" s="12" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:47" ht="66.599999999999994" thickBot="1">
@@ -1809,7 +1821,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>21</v>
@@ -1822,49 +1834,49 @@
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="2" t="s">
-        <v>167</v>
+        <v>213</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>168</v>
+      <c r="K12" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="S12" s="9" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="V12" s="11"/>
       <c r="W12" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:47" ht="93" thickBot="1">
       <c r="A13" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>24</v>
@@ -1876,34 +1888,34 @@
         <v>25</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>170</v>
+        <v>216</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>171</v>
+      <c r="K13" s="16" t="s">
+        <v>215</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="V13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:47" ht="40.200000000000003" thickBot="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" ht="42" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -1911,68 +1923,59 @@
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>35</v>
+        <v>17</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="N14" s="11"/>
       <c r="O14" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:47" ht="97.2" thickBot="1">
       <c r="A15" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>40</v>
+        <v>207</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>0</v>
@@ -1999,83 +2002,90 @@
         <v>4</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:47" ht="40.200000000000003" thickBot="1">
       <c r="A16" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>200</v>
+      <c r="I16" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>29</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="V16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="53.4" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="Q17" s="3" t="s">
         <v>12</v>
@@ -2084,16 +2094,16 @@
         <v>13</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="V17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="119.4" thickBot="1">
@@ -2107,159 +2117,150 @@
         <v>23</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11" t="s">
-        <v>177</v>
+      <c r="J18" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="R18" s="7" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="S18" s="8" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="V18" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="96" thickBot="1">
       <c r="E19" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>161</v>
+        <v>219</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="R19" s="7" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="S19" s="8" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="V19" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="79.8" thickBot="1">
       <c r="E20" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>166</v>
+        <v>58</v>
       </c>
       <c r="U20" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="V20" s="4" t="s">
         <v>22</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="93" thickBot="1">
-      <c r="I21" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>178</v>
+      <c r="I21" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11" t="s">
+        <v>168</v>
       </c>
       <c r="Q21" s="10" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="R21" s="11"/>
       <c r="S21" s="12" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="66.599999999999994" thickBot="1">
       <c r="E22" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>211</v>
+        <v>3</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>212</v>
+        <v>158</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="Q22" s="13" t="s">
         <v>3</v>
       </c>
       <c r="R22" s="14" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="S22" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="40.200000000000003" thickBot="1">
@@ -2267,100 +2268,111 @@
         <v>3</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="I23" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="Q23" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R23" s="14" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="S23" s="15" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="V23" s="11"/>
       <c r="W23" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="40.200000000000003" thickBot="1">
+      <c r="E24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" ht="53.4" thickBot="1">
-      <c r="E24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="G24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11" t="s">
-        <v>62</v>
+        <v>53</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="Q24" s="6" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="R24" s="7" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="V24" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="132.6" thickBot="1">
       <c r="E25" s="3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>3</v>
+        <v>201</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>202</v>
       </c>
       <c r="Q25" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="S25" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="R25" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="S25" s="8" t="s">
-        <v>203</v>
-      </c>
       <c r="U25" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="27" thickBot="1">
@@ -2368,152 +2380,176 @@
         <v>0</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J26" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q26" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="K26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q26" s="6" t="s">
-        <v>195</v>
-      </c>
       <c r="R26" s="7" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="S26" s="4" t="s">
         <v>34</v>
       </c>
       <c r="U26" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="V26" s="4" t="s">
         <v>17</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" ht="40.200000000000003" thickBot="1">
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="I27" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>172</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="53.4" thickBot="1">
+      <c r="E27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>7</v>
       </c>
       <c r="S27" s="7"/>
       <c r="U27" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="V27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" ht="40.200000000000003" thickBot="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="27" thickBot="1">
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="I28" s="3" t="s">
-        <v>210</v>
+        <v>3</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="R28" s="7" t="s">
         <v>13</v>
       </c>
       <c r="S28" s="7"/>
       <c r="U28" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="V28" s="4" t="s">
         <v>17</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="27" thickBot="1">
       <c r="I29" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="U29" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="V29" s="4" t="s">
         <v>17</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="40.200000000000003" thickBot="1">
       <c r="I30" s="3" t="s">
-        <v>31</v>
+        <v>161</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>32</v>
+        <v>164</v>
       </c>
       <c r="U30" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="V30" s="4" t="s">
         <v>17</v>
       </c>
       <c r="W30" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="40.200000000000003" thickBot="1">
+      <c r="I31" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="Q31"/>
       <c r="U31" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="V31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="17:17" ht="15">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="13.8" thickBot="1">
+      <c r="I32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="9:17" ht="15.6" thickBot="1">
+      <c r="I33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="Q33"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project - SQL Design change
</commit_message>
<xml_diff>
--- a/doc/SQL_design.xlsx
+++ b/doc/SQL_design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="269">
   <si>
     <t>item_id</t>
   </si>
@@ -152,15 +152,6 @@
     <t>庫存數量</t>
   </si>
   <si>
-    <t>low_stock_threshold</t>
-  </si>
-  <si>
-    <t>庫存警戒值</t>
-  </si>
-  <si>
-    <t>last_updated</t>
-  </si>
-  <si>
     <t>tag_id</t>
   </si>
   <si>
@@ -216,9 +207,6 @@
   </si>
   <si>
     <t>商品主表</t>
-  </si>
-  <si>
-    <t>庫存管理</t>
   </si>
   <si>
     <t xml:space="preserve">item_tags </t>
@@ -692,10 +680,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>INT (CPK FK)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>combo_item_group</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -733,10 +717,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>inventory</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>option_group</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -774,6 +754,280 @@
   </si>
   <si>
     <t>INT (CPK FK)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>material_id</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>材料名稱</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>單位（如g, ml, pcs等）</t>
+  </si>
+  <si>
+    <t>DECIMAL(10,2)</t>
+  </si>
+  <si>
+    <t>min_stock_alert</t>
+  </si>
+  <si>
+    <t>最低庫存警示值</t>
+  </si>
+  <si>
+    <t>更新時間</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF424242"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>商品</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF424242"/>
+        <rFont val="Siemens Sans Global"/>
+      </rPr>
+      <t xml:space="preserve"> ID</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>material</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>材料/原料</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>商家ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>材料ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT (CPK)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT (CPK FK)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>材料ID（外鍵）</t>
+  </si>
+  <si>
+    <t>quantity_needed</t>
+  </si>
+  <si>
+    <t>需要用量</t>
+  </si>
+  <si>
+    <t>option_id</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品選項ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>材料ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>movement_id</t>
+  </si>
+  <si>
+    <t>movement_type</t>
+  </si>
+  <si>
+    <t>異動類型（進貨、銷售、調整、報廢等）</t>
+  </si>
+  <si>
+    <t>異動數量</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>備註</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>商家</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Siemens Sans Global"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>異動紀錄</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Siemens Sans Global"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>材料</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Siemens Sans Global"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT (FK)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase_id</t>
+  </si>
+  <si>
+    <t>supplier</t>
+  </si>
+  <si>
+    <t>供應商名稱</t>
+  </si>
+  <si>
+    <t>狀態（預設PENDING）</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>進貨單</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Siemens Sans Global"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT (CPK)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase_order</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>進貨單</t>
+  </si>
+  <si>
+    <t>inventory_movement</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>庫存異動紀錄</t>
+  </si>
+  <si>
+    <t>option_material</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品選項-材料配方</t>
+  </si>
+  <si>
+    <t>menu_item_material</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品-材料配方</t>
+  </si>
+  <si>
+    <t>進貨數量</t>
+  </si>
+  <si>
+    <t>單價</t>
+  </si>
+  <si>
+    <t>purchase_order_item</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>進貨單明細</t>
+  </si>
+  <si>
+    <t>movement_id</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT (FK)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -781,7 +1035,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -818,6 +1072,12 @@
       <color rgb="FF424242"/>
       <name val="細明體"/>
       <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
       <charset val="136"/>
     </font>
   </fonts>
@@ -871,7 +1131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -920,6 +1180,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1201,32 +1470,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU33"/>
+  <dimension ref="A1:AU46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="11.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="8.75" style="2"/>
-    <col min="3" max="3" width="10.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.375" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.75" style="2"/>
     <col min="5" max="5" width="16.125" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="2" customWidth="1"/>
-    <col min="7" max="8" width="8.75" style="2"/>
+    <col min="7" max="7" width="14" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.75" style="2"/>
     <col min="9" max="9" width="15.5" style="2" customWidth="1"/>
     <col min="10" max="10" width="12" style="2" customWidth="1"/>
     <col min="11" max="11" width="12.125" style="2" customWidth="1"/>
     <col min="12" max="12" width="8.75" style="2"/>
     <col min="13" max="13" width="21.125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.75" style="2" customWidth="1"/>
-    <col min="15" max="16" width="8.75" style="2"/>
+    <col min="14" max="14" width="17.125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.75" style="2" customWidth="1"/>
+    <col min="16" max="16" width="8.75" style="2"/>
     <col min="17" max="17" width="19.125" style="2" customWidth="1"/>
-    <col min="18" max="20" width="8.75" style="2"/>
+    <col min="18" max="18" width="8.75" style="2"/>
+    <col min="19" max="19" width="18.375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="8.75" style="2"/>
     <col min="21" max="21" width="21.75" style="2" customWidth="1"/>
-    <col min="22" max="24" width="8.75" style="2"/>
+    <col min="22" max="22" width="8.75" style="2"/>
+    <col min="23" max="23" width="19.125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="8.75" style="2"/>
     <col min="25" max="25" width="12.125" style="2" customWidth="1"/>
     <col min="26" max="26" width="10.625" style="2" customWidth="1"/>
     <col min="27" max="28" width="8.75" style="2"/>
@@ -1251,46 +1526,46 @@
   <sheetData>
     <row r="1" spans="1:47" ht="56.55" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F1" s="11"/>
       <c r="G1" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J1" s="11"/>
       <c r="K1" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="R1" s="11"/>
       <c r="S1" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="V1" s="11"/>
       <c r="W1" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:47" ht="40.200000000000003" thickBot="1">
@@ -1307,7 +1582,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>5</v>
@@ -1317,37 +1592,37 @@
         <v>3</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>5</v>
+      <c r="N2" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>227</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="X2" s="4"/>
     </row>
@@ -1359,13 +1634,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>2</v>
@@ -1375,28 +1650,28 @@
         <v>14</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>2</v>
+      <c r="M3" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>228</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>3</v>
@@ -1409,7 +1684,7 @@
       </c>
       <c r="X3" s="4"/>
     </row>
-    <row r="4" spans="1:47" ht="93" thickBot="1">
+    <row r="4" spans="1:47" ht="53.4" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1417,7 +1692,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -1438,44 +1713,44 @@
       <c r="K4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>41</v>
+      <c r="M4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>216</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:47" ht="40.200000000000003" thickBot="1">
+    <row r="5" spans="1:47" ht="28.2" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
@@ -1496,44 +1771,44 @@
       <c r="K5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>43</v>
+      <c r="M5" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>219</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="X5" s="4"/>
     </row>
-    <row r="6" spans="1:47" ht="79.8" thickBot="1">
+    <row r="6" spans="1:47" ht="53.4" thickBot="1">
       <c r="A6" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -1542,7 +1817,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="3" t="s">
@@ -1554,32 +1829,32 @@
       <c r="K6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>25</v>
+      <c r="M6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="R6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:47" ht="27" thickBot="1">
@@ -1604,26 +1879,35 @@
       <c r="H7" s="5"/>
       <c r="I7" s="1"/>
       <c r="J7" s="4"/>
+      <c r="M7" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>222</v>
+      </c>
       <c r="Q7" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="V7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:47" ht="79.8" thickBot="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" ht="53.4" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1644,138 +1928,140 @@
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="11" t="s">
-        <v>210</v>
+        <v>61</v>
       </c>
       <c r="J8" s="11"/>
-      <c r="K8" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11" t="s">
-        <v>66</v>
+      <c r="K8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="V8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="Y8" s="3"/>
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
     </row>
-    <row r="9" spans="1:47" ht="79.8" thickBot="1">
+    <row r="9" spans="1:47" ht="40.200000000000003" thickBot="1">
       <c r="E9" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="O9" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="M9" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>23</v>
+      </c>
       <c r="Q9" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="V9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:47" ht="93" thickBot="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" ht="40.200000000000003" thickBot="1">
       <c r="A10" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="3" t="s">
-        <v>161</v>
+        <v>42</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>157</v>
+        <v>1</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>223</v>
       </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="7"/>
       <c r="AU10" s="7"/>
     </row>
-    <row r="11" spans="1:47" ht="40.200000000000003" thickBot="1">
+    <row r="11" spans="1:47" ht="28.2" thickBot="1">
       <c r="A11" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>19</v>
@@ -1788,32 +2074,23 @@
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="3" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q11" s="10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="R11" s="11"/>
       <c r="S11" s="12" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:47" ht="66.599999999999994" thickBot="1">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" ht="40.200000000000003" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1821,7 +2098,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>21</v>
@@ -1833,50 +2110,48 @@
         <v>23</v>
       </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="2" t="s">
-        <v>213</v>
+      <c r="I12" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O12" s="4" t="s">
-        <v>49</v>
+      <c r="K12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19" t="s">
+        <v>262</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="S12" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="V12" s="11"/>
       <c r="W12" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:47" ht="93" thickBot="1">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" ht="40.200000000000003" thickBot="1">
       <c r="A13" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>24</v>
@@ -1887,35 +2162,35 @@
       <c r="G13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>215</v>
+      <c r="M13" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>227</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="V13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:47" ht="42" thickBot="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" ht="27" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -1923,68 +2198,77 @@
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11" t="s">
-        <v>68</v>
+        <v>79</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>237</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="V14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:47" ht="97.2" thickBot="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" ht="55.8" thickBot="1">
       <c r="A15" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="M15" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O15" s="4" t="s">
-        <v>2</v>
+      <c r="K15" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="N15" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O15" s="17" t="s">
+        <v>236</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>0</v>
@@ -2007,85 +2291,78 @@
     </row>
     <row r="16" spans="1:47" ht="40.200000000000003" thickBot="1">
       <c r="A16" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N16" s="4" t="s">
+      <c r="I16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O16" s="4" t="s">
-        <v>46</v>
+      <c r="K16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="N16" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>233</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>29</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="V16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="53.4" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="Q17" s="3" t="s">
         <v>12</v>
@@ -2094,19 +2371,19 @@
         <v>13</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="V17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="119.4" thickBot="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="53.4" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -2117,78 +2394,92 @@
         <v>23</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="J18" s="11"/>
+      <c r="K18" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>162</v>
+      <c r="M18" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19" t="s">
+        <v>260</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="R18" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="S18" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="V18" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="96" thickBot="1">
       <c r="E19" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>219</v>
+        <v>154</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="N19" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>227</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="R19" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="S19" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="V19" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="79.8" thickBot="1">
@@ -2199,65 +2490,103 @@
         <v>7</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="N20" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>235</v>
       </c>
       <c r="U20" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="V20" s="4" t="s">
         <v>22</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="93" thickBot="1">
-      <c r="I21" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11" t="s">
-        <v>168</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="40.200000000000003" thickBot="1">
+      <c r="I21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="M21" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="N21" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O21" s="17" t="s">
+        <v>228</v>
       </c>
       <c r="Q21" s="10" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="R21" s="11"/>
       <c r="S21" s="12" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="V21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="66.599999999999994" thickBot="1">
       <c r="E22" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>3</v>
+        <v>155</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="M22" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>233</v>
       </c>
       <c r="Q22" s="13" t="s">
         <v>3</v>
       </c>
       <c r="R22" s="14" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="S22" s="14" t="s">
         <v>39</v>
@@ -2268,143 +2597,166 @@
         <v>3</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>161</v>
+      <c r="I23" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>162</v>
+        <v>7</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>209</v>
       </c>
       <c r="Q23" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="R23" s="14" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="S23" s="15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="V23" s="11"/>
       <c r="W23" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" ht="40.200000000000003" thickBot="1">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="42" thickBot="1">
       <c r="E24" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>169</v>
+        <v>17</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="N24" s="11"/>
+      <c r="O24" s="12" t="s">
+        <v>258</v>
       </c>
       <c r="Q24" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="R24" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="V24" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="W24" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="132.6" thickBot="1">
+    <row r="25" spans="1:23" ht="56.4" customHeight="1" thickBot="1">
       <c r="E25" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="I25" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>202</v>
+      <c r="M25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N25" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="Q25" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="R25" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="S25" s="8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="U25" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" ht="27" thickBot="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="28.2" thickBot="1">
       <c r="E26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="J26" s="11"/>
+      <c r="K26" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="Q26" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="R26" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="S26" s="4" t="s">
         <v>34</v>
       </c>
       <c r="U26" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="V26" s="4" t="s">
         <v>17</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" ht="53.4" thickBot="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="27" thickBot="1">
       <c r="E27" s="3" t="s">
         <v>36</v>
       </c>
@@ -2414,143 +2766,397 @@
       <c r="G27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I27" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11" t="s">
-        <v>59</v>
+      <c r="I27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>7</v>
       </c>
       <c r="S27" s="7"/>
       <c r="U27" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="V27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" ht="27" thickBot="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="40.200000000000003" thickBot="1">
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="I28" s="3" t="s">
-        <v>3</v>
+        <v>157</v>
       </c>
       <c r="J28" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="K28" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="K28" s="4" t="s">
-        <v>5</v>
+      <c r="M28" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="R28" s="7" t="s">
         <v>13</v>
       </c>
       <c r="S28" s="7"/>
       <c r="U28" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="V28" s="4" t="s">
         <v>17</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="27" thickBot="1">
       <c r="I29" s="3" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>177</v>
+        <v>213</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>34</v>
+        <v>2</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="U29" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="V29" s="4" t="s">
         <v>17</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" ht="40.200000000000003" thickBot="1">
-      <c r="I30" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>164</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="27" thickBot="1">
+      <c r="M30" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="U30" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="V30" s="4" t="s">
         <v>17</v>
       </c>
       <c r="W30" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="40.200000000000003" thickBot="1">
-      <c r="I31" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>35</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="27" thickBot="1">
+      <c r="I31" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="Q31"/>
       <c r="U31" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="V31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" ht="13.8" thickBot="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="27" thickBot="1">
       <c r="I32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="9:17" ht="27" thickBot="1">
+      <c r="I33" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="M33" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="N33" s="11"/>
+      <c r="O33" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q33"/>
+    </row>
+    <row r="34" spans="9:17" ht="27" thickBot="1">
+      <c r="I34" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="35" spans="9:17" ht="42" thickBot="1">
+      <c r="I35" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="N35" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="36" spans="9:17">
+      <c r="M36" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="37" spans="9:17" ht="52.8">
+      <c r="I37" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="9:17" ht="27" thickBot="1">
+      <c r="I38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="9:17" ht="13.8" thickBot="1">
+      <c r="I39" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="9:17" ht="27" thickBot="1">
+      <c r="I40" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="M40" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="N40" s="11"/>
+      <c r="O40" s="12" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="41" spans="9:17" ht="40.200000000000003" thickBot="1">
+      <c r="I41" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N41" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="9:17" ht="14.4" thickBot="1">
+      <c r="I42" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J42" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K42" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="9:17" ht="15.6" thickBot="1">
-      <c r="I33" s="3" t="s">
+      <c r="M42" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="N42" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="43" spans="9:17" ht="14.4" thickBot="1">
+      <c r="I43" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J43" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K43" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q33"/>
+      <c r="M43" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="9:17" ht="13.8">
+      <c r="M44" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="N44" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="9:17">
+      <c r="M45" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="9:17">
+      <c r="M46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>264</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>